<commit_message>
Trying to get excel sync to work.
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/Platform/Ordnance_and_Missiles/DoD_Ordnance_and_Missiles_Contracts.xlsx
+++ b/Output/AcqTrends/Platform/Ordnance_and_Missiles/DoD_Ordnance_and_Missiles_Contracts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Greg\Repositories\Vendor\Output\AcqTrends\Platform\Ordnance_and_Missiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2755E0B7-435C-4873-A710-3E4909172BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68B4E39-7EF7-4806-8646-5D134B594E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -992,8 +992,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.0,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1035,11 +1036,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9602,7 +9605,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10678,15 +10681,15 @@
         <f t="shared" si="2"/>
         <v>AMRAAM</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="5">
         <f t="shared" si="3"/>
         <v>1373740839.41664</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="5">
         <f t="shared" si="4"/>
         <v>1473439671.3803999</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="5">
         <f t="shared" si="5"/>
         <v>1189368825.4702001</v>
       </c>
@@ -10797,15 +10800,15 @@
         <f t="shared" si="2"/>
         <v>BGM-109 TOMAHAWK</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -10882,19 +10885,19 @@
         <f t="shared" si="2"/>
         <v>GMLRS</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="5">
         <f t="shared" si="3"/>
         <v>110377116.851156</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <f t="shared" si="4"/>
         <v>1810181640.9732499</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="4">
         <f t="shared" si="5"/>
         <v>1267113243.3921001</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <f t="shared" si="6"/>
         <v>2182425659.69138</v>
       </c>
@@ -10998,15 +11001,15 @@
         <f t="shared" si="2"/>
         <v>JASSM</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="5">
         <f t="shared" si="3"/>
         <v>100824090.085522</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="5">
         <f t="shared" si="4"/>
         <v>1157018668.5292699</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="5">
         <f t="shared" si="5"/>
         <v>980912151.5704</v>
       </c>
@@ -11109,15 +11112,15 @@
         <f t="shared" si="2"/>
         <v>JDAM</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="5">
         <f t="shared" si="3"/>
         <v>320101497.03950399</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="5">
         <f t="shared" si="4"/>
         <v>466465647.229366</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="5">
         <f t="shared" si="5"/>
         <v>283583798.29640001</v>
       </c>
@@ -11220,15 +11223,15 @@
         <f t="shared" si="2"/>
         <v>Other Labeled Project</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="5">
         <f t="shared" si="3"/>
         <v>2116241367.48086</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="5">
         <f t="shared" si="4"/>
         <v>1561002770.95123</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="5">
         <f t="shared" si="5"/>
         <v>1021941736.6932</v>
       </c>
@@ -11339,15 +11342,15 @@
         <f t="shared" si="2"/>
         <v>TACTICAL TOMAHAWK</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="5">
         <f t="shared" si="3"/>
         <v>371288883.32419902</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="5">
         <f t="shared" si="4"/>
         <v>525719026.80893898</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="5">
         <f t="shared" si="5"/>
         <v>596305484.42850006</v>
       </c>
@@ -11450,15 +11453,15 @@
         <f t="shared" si="2"/>
         <v>TRIDENT II MISSILE</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="5">
         <f t="shared" si="3"/>
         <v>2712629575.7695298</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="4">
         <f t="shared" si="4"/>
         <v>3127387813.9230599</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="4">
         <f t="shared" si="5"/>
         <v>2517048390.0236001</v>
       </c>
@@ -11569,15 +11572,15 @@
         <f t="shared" si="2"/>
         <v>UGM-96 TRIDENT</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="5">
         <f t="shared" si="3"/>
         <v>-832231.36047205899</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -11686,15 +11689,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="5">
         <f t="shared" si="3"/>
         <v>8789336728.2479706</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="5">
         <f t="shared" si="4"/>
         <v>13372035247.6985</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="5">
         <f t="shared" si="5"/>
         <v>12623676860.4419</v>
       </c>
@@ -11802,15 +11805,15 @@
         <f t="shared" si="2"/>
         <v>Grand Total</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="5">
         <f t="shared" si="3"/>
         <v>15893707866.85491</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="5">
         <f t="shared" si="4"/>
         <v>23493250487.494015</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="5">
         <f t="shared" si="5"/>
         <v>20479950490.316299</v>
       </c>
@@ -11954,7 +11957,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23:D23"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13232,19 +13235,19 @@
         <v>AMMUNITION, THROUGH
 30 MM</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="5">
         <f t="shared" si="3"/>
         <v>796854869.84024405</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="5">
         <f t="shared" si="4"/>
         <v>712674777.29412603</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="5">
         <f t="shared" si="5"/>
         <v>723887533.99829996</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="5">
         <f t="shared" si="6"/>
         <v>135084306.01576</v>
       </c>
@@ -13351,19 +13354,19 @@
         <f t="shared" si="2"/>
         <v>BOMBS</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="5">
         <f t="shared" si="3"/>
         <v>738054640.06627202</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="5">
         <f t="shared" si="4"/>
         <v>1939773496.18558</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="5">
         <f t="shared" si="5"/>
         <v>1273626107.9995</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="5">
         <f t="shared" si="6"/>
         <v>1037613049.13472</v>
       </c>
@@ -13471,19 +13474,19 @@
         <v>GUIDED MISSILE
 COMPONENTS</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="5">
         <f t="shared" si="3"/>
         <v>1214251045.94874</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="5">
         <f t="shared" si="4"/>
         <v>1686361042.60357</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="5">
         <f t="shared" si="5"/>
         <v>1503699709.4323001</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="5">
         <f t="shared" si="6"/>
         <v>1064751511.2828</v>
       </c>
@@ -13591,19 +13594,19 @@
         <v>GUIDED MISSILE
 SUBSYSTEMS</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="5">
         <f t="shared" si="3"/>
         <v>876249178.76871705</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="5">
         <f t="shared" si="4"/>
         <v>698701308.63821304</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="5">
         <f t="shared" si="5"/>
         <v>1027089280.2831</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="5">
         <f t="shared" si="6"/>
         <v>301920671.15798903</v>
       </c>
@@ -13711,19 +13714,19 @@
         <v>GUIDED MISSILE
 SYSTEMS, COMPLETE</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="5">
         <f t="shared" si="3"/>
         <v>236909652.298094</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="5">
         <f t="shared" si="4"/>
         <v>1870990141.3524001</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="5">
         <f t="shared" si="5"/>
         <v>1672750360.2051001</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="5">
         <f t="shared" si="6"/>
         <v>1950770296.01597</v>
       </c>
@@ -13830,19 +13833,19 @@
         <f t="shared" si="2"/>
         <v>GUIDED MISSILES</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="5">
         <f t="shared" si="3"/>
         <v>4587694143.6237297</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="4">
         <f t="shared" si="4"/>
         <v>6557652134.2112103</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="4">
         <f t="shared" si="5"/>
         <v>5058661429.5676003</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="5">
         <f t="shared" si="6"/>
         <v>4611965192.0318699</v>
       </c>
@@ -13949,19 +13952,19 @@
         <f t="shared" si="2"/>
         <v>GUNS, THROUGH 30 MM</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="5">
         <f t="shared" si="3"/>
         <v>329763749.764992</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="5">
         <f t="shared" si="4"/>
         <v>320391417.08895397</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="5">
         <f t="shared" si="5"/>
         <v>449297694.79259998</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="5">
         <f t="shared" si="6"/>
         <v>164595881.79418001</v>
       </c>
@@ -14069,19 +14072,19 @@
         <v>LAUNCHERS, GUIDED
 MISSILE</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="5">
         <f t="shared" si="3"/>
         <v>597714290.22491097</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="5">
         <f t="shared" si="4"/>
         <v>702942435.149333</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="5">
         <f t="shared" si="5"/>
         <v>349836741.59320003</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="5">
         <f t="shared" si="6"/>
         <v>1129768986.30878</v>
       </c>
@@ -14189,19 +14192,19 @@
         <v>MISCELLANEOUS
 WEAPONS</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="5">
         <f t="shared" si="3"/>
         <v>626111909.35423505</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="5">
         <f t="shared" si="4"/>
         <v>396402593.72911</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="5">
         <f t="shared" si="5"/>
         <v>519969539.8337</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="5">
         <f t="shared" si="6"/>
         <v>355869798.43852901</v>
       </c>
@@ -14308,19 +14311,19 @@
         <f t="shared" si="2"/>
         <v>Other Labeled PSC</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="5">
         <f t="shared" si="3"/>
         <v>5548318782.18328</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="5">
         <f t="shared" si="4"/>
         <v>8079801803.3554497</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="5">
         <f t="shared" si="5"/>
         <v>7397840950.1160002</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="5">
         <f t="shared" si="6"/>
         <v>6428770764.6521196</v>
       </c>
@@ -14429,19 +14432,19 @@
 SVCS/GUIDED
 MISSILES</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="5">
         <f t="shared" si="3"/>
         <v>341785604.78168601</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="5">
         <f t="shared" si="4"/>
         <v>527559337.88604301</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="5">
         <f t="shared" si="5"/>
         <v>503291142.49489999</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="5">
         <f t="shared" si="6"/>
         <v>247861303.130622</v>
       </c>
@@ -14548,19 +14551,19 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -14622,19 +14625,19 @@
         <f t="shared" si="2"/>
         <v>Grand Total</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="5">
         <f t="shared" si="3"/>
         <v>15893707866.854902</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="5">
         <f t="shared" si="4"/>
         <v>23493250487.493992</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="5">
         <f t="shared" si="5"/>
         <v>20479950490.316303</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="5">
         <f t="shared" si="6"/>
         <v>17428971759.963341</v>
       </c>

</xml_diff>